<commit_message>
reglas y buena fe
</commit_message>
<xml_diff>
--- a/Documentos/buenaFe/Lista Buena Fe Futbol 5.xlsx
+++ b/Documentos/buenaFe/Lista Buena Fe Futbol 5.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\caraya\reglamentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\COPA CORRIENTES DIVERSA\Listas de Buena Fe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096EC8A1-12DE-42B4-9E16-CEC0B68B6362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0C2568-DFD6-41D0-9E32-07E87500A7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nombre del Club/Equipo</t>
   </si>
@@ -61,15 +61,6 @@
     <t>LISTADO DE BUENA FE CUERPO TÉCNICO</t>
   </si>
   <si>
-    <t>LISTADO DE BUENA FE JUGADORES**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(*) EN CASO LLUEVA, LOS PARTIDOS DE LA CANCHA DESCUBIERTA PASARÍAN A LA CUBIERTA, EXTENDIÉNDOSE O MODIFICANDÓSE </t>
-  </si>
-  <si>
-    <t>EL CRONOGRAMA (**) MÍNIMO DE 6 PERSONAS PARA INSCRIBIRSE. EL C. T. DEBE ESTAR DENTRO DEL LISTADO DE BUENA FE</t>
-  </si>
-  <si>
     <t>MÉDICO</t>
   </si>
   <si>
@@ -79,7 +70,13 @@
     <t>"COPA CORRIENTES DIVERSA"</t>
   </si>
   <si>
-    <t>10,11 y 12 de Febrero  de 2024 - Corrientes -Argentina</t>
+    <t>Mixta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LISTADO DE BUENA FE </t>
+  </si>
+  <si>
+    <t>10, 11, 12 y 13 de Febrero  de 2024 - Corrientes - Argentina.</t>
   </si>
 </sst>
 </file>
@@ -240,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -280,17 +277,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -321,19 +307,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -423,19 +396,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -524,15 +484,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -547,7 +498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -562,13 +513,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -577,10 +522,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -595,162 +540,152 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -878,15 +813,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1244019</xdr:colOff>
+      <xdr:colOff>1132809</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>69395</xdr:rowOff>
+      <xdr:rowOff>183694</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1310158</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>90354</xdr:rowOff>
+      <xdr:colOff>1319683</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -915,8 +850,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6340083" y="69395"/>
-          <a:ext cx="1412439" cy="1412439"/>
+          <a:off x="5923884" y="183694"/>
+          <a:ext cx="1453699" cy="1549855"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -928,22 +863,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>58135</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>151679</xdr:rowOff>
+      <xdr:colOff>420085</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>113579</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02F4FCAE-B1A2-4327-909D-C1E0098AD437}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{469005F8-7022-40D5-BA1A-4BF811F01AB8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -959,7 +894,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2276475" y="9315450"/>
+          <a:off x="2638425" y="8677275"/>
           <a:ext cx="2572735" cy="475529"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -973,7 +908,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="B18:F37" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="B18:F33" headerRowDxfId="2">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Orden" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="APELLIDOS" dataDxfId="0"/>
@@ -1186,10 +1121,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H238"/>
+  <dimension ref="A1:H235"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1205,1101 +1140,1059 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A1" s="47"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="50"/>
+      <c r="A1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A2" s="51"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="54"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="50"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A3" s="51"/>
-      <c r="B3" s="74" t="s">
+      <c r="A3" s="47"/>
+      <c r="B3" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="50"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A4" s="47"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="50"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A5" s="47"/>
+      <c r="B5" s="69">
+        <v>2024</v>
+      </c>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="50"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A6" s="47"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="50"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A7" s="47"/>
+      <c r="B7" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="50"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A8" s="47"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="50"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A9" s="47"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="54"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A4" s="51"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="54"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A5" s="51"/>
-      <c r="B5" s="74">
-        <v>2024</v>
-      </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="54"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A6" s="51"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="54"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A7" s="51"/>
-      <c r="B7" s="75" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="54"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A8" s="51"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="54"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="80" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="54"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="50"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A10" s="51"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="54"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="50"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A11" s="51"/>
-      <c r="B11" s="81" t="s">
+      <c r="A11" s="47"/>
+      <c r="B11" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="45"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="41"/>
       <c r="E11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="54"/>
+      <c r="G11" s="50"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A12" s="51"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="54"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="50"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A13" s="51"/>
-      <c r="B13" s="81" t="s">
+      <c r="A13" s="47"/>
+      <c r="B13" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="44"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="40"/>
       <c r="E13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="54"/>
+      <c r="F13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="50"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="54"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="50"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A15" s="51"/>
-      <c r="B15" s="81" t="s">
+      <c r="A15" s="47"/>
+      <c r="B15" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="82"/>
+      <c r="C15" s="76"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="54"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="50"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A16" s="51"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="54"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A17" s="51"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="54"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="33"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A18" s="51"/>
-      <c r="B18" s="27" t="s">
+      <c r="A18" s="47"/>
+      <c r="B18" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="54"/>
+      <c r="G18" s="50"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A19" s="51"/>
-      <c r="B19" s="26">
+      <c r="A19" s="47"/>
+      <c r="B19" s="23">
         <v>1</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="54"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="50"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A20" s="51"/>
-      <c r="B20" s="13">
+      <c r="A20" s="47"/>
+      <c r="B20" s="11">
         <v>2</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="54"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="50"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A21" s="51"/>
-      <c r="B21" s="13">
+      <c r="A21" s="47"/>
+      <c r="B21" s="11">
         <v>3</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="54"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="50"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A22" s="51"/>
-      <c r="B22" s="13">
+      <c r="A22" s="47"/>
+      <c r="B22" s="11">
         <v>4</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="54"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="50"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A23" s="51"/>
-      <c r="B23" s="13">
+      <c r="A23" s="47"/>
+      <c r="B23" s="11">
         <v>5</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="54"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="50"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A24" s="51"/>
-      <c r="B24" s="13">
+      <c r="A24" s="47"/>
+      <c r="B24" s="11">
         <v>6</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="54"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="50"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A25" s="51"/>
-      <c r="B25" s="13">
+      <c r="A25" s="47"/>
+      <c r="B25" s="11">
         <v>7</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="54"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="50"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A26" s="51"/>
-      <c r="B26" s="13">
+      <c r="A26" s="47"/>
+      <c r="B26" s="11">
         <v>8</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="54"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="50"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A27" s="51"/>
-      <c r="B27" s="13">
+      <c r="A27" s="47"/>
+      <c r="B27" s="11">
         <v>9</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="54"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="50"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A28" s="51"/>
-      <c r="B28" s="13">
+      <c r="A28" s="47"/>
+      <c r="B28" s="11">
         <v>10</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="54"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="50"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A29" s="51"/>
-      <c r="B29" s="14">
+      <c r="A29" s="47"/>
+      <c r="B29" s="12">
         <v>11</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="6"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="54"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="50"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A30" s="51"/>
-      <c r="B30" s="13">
+      <c r="A30" s="47"/>
+      <c r="B30" s="11">
         <v>12</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="6"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="54"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="50"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A31" s="51"/>
-      <c r="B31" s="14">
+      <c r="A31" s="47"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="19"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="50"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A32" s="47"/>
+      <c r="B32" s="16">
+        <v>1</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="50"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A33" s="47"/>
+      <c r="B33" s="12">
+        <v>2</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="50"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A34" s="47"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="50"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A35" s="47"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="50"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A36" s="47"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="50"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A37" s="60"/>
+      <c r="B37" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="50"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A38" s="60"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="61"/>
+      <c r="G38" s="50"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A39" s="60"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="61"/>
+      <c r="G39" s="50"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A40" s="60"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="61"/>
+      <c r="G40" s="50"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A41" s="60"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="50"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A42" s="60"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="54"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A32" s="51"/>
-      <c r="B32" s="14">
-        <v>14</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="54"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A33" s="51"/>
-      <c r="B33" s="18">
-        <v>15</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="54"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A34" s="51"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="22"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="54"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A35" s="51"/>
-      <c r="B35" s="19">
-        <v>1</v>
-      </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="54"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A36" s="51"/>
-      <c r="B36" s="14">
-        <v>2</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="54"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A37" s="51"/>
-      <c r="B37" s="14">
-        <v>3</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="54"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A38" s="51"/>
-      <c r="B38" s="78" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="79"/>
-      <c r="D38" s="79"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="79"/>
-      <c r="G38" s="54"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A39" s="51"/>
-      <c r="B39" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="63"/>
-      <c r="D39" s="63"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="63"/>
-      <c r="G39" s="54"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A40" s="64"/>
-      <c r="B40" s="65"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="65"/>
-      <c r="E40" s="66"/>
-      <c r="F40" s="65"/>
-      <c r="G40" s="54"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A41" s="64"/>
-      <c r="B41" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="65"/>
-      <c r="D41" s="65"/>
-      <c r="E41" s="66"/>
-      <c r="F41" s="65"/>
-      <c r="G41" s="54"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A42" s="64"/>
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="66"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="54"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="50"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A43" s="64"/>
-      <c r="B43" s="65"/>
-      <c r="C43" s="65"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="66"/>
-      <c r="F43" s="65"/>
-      <c r="G43" s="54"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A44" s="64"/>
-      <c r="B44" s="65"/>
-      <c r="C44" s="65"/>
-      <c r="D44" s="65"/>
-      <c r="E44" s="65"/>
-      <c r="F44" s="65"/>
-      <c r="G44" s="54"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A45" s="64"/>
-      <c r="B45" s="65"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="65"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="54"/>
+      <c r="A43" s="60"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="50"/>
+    </row>
+    <row r="44" spans="1:7" ht="34.5" customHeight="1">
+      <c r="A44" s="60"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="65"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A45" s="66"/>
+      <c r="E45" s="7"/>
+      <c r="G45" s="67"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A46" s="64"/>
-      <c r="B46" s="65"/>
-      <c r="C46" s="65"/>
-      <c r="D46" s="65"/>
-      <c r="E46" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="F46" s="65"/>
-      <c r="G46" s="54"/>
-    </row>
-    <row r="47" spans="1:7" ht="34.5" customHeight="1">
-      <c r="A47" s="64"/>
-      <c r="B47" s="76"/>
-      <c r="C47" s="76"/>
-      <c r="D47" s="76"/>
-      <c r="E47" s="76"/>
-      <c r="F47" s="76"/>
-      <c r="G47" s="69"/>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A48" s="70"/>
-      <c r="B48" s="71"/>
-      <c r="C48" s="71"/>
-      <c r="D48" s="71"/>
-      <c r="E48" s="72"/>
-      <c r="F48" s="71"/>
-      <c r="G48" s="73"/>
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" customHeight="1">
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1">
+      <c r="E48" s="7"/>
     </row>
     <row r="49" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E49" s="9"/>
+      <c r="E49" s="7"/>
     </row>
     <row r="50" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E50" s="9"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E51" s="9"/>
+      <c r="E51" s="7"/>
     </row>
     <row r="52" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E52" s="9"/>
+      <c r="E52" s="7"/>
     </row>
     <row r="53" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E53" s="9"/>
+      <c r="E53" s="7"/>
     </row>
     <row r="54" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E54" s="9"/>
+      <c r="E54" s="7"/>
     </row>
     <row r="55" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E55" s="9"/>
+      <c r="E55" s="7"/>
     </row>
     <row r="56" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E56" s="9"/>
+      <c r="E56" s="7"/>
     </row>
     <row r="57" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E57" s="9"/>
+      <c r="E57" s="7"/>
     </row>
     <row r="58" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E58" s="9"/>
+      <c r="E58" s="7"/>
     </row>
     <row r="59" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E59" s="9"/>
+      <c r="E59" s="7"/>
     </row>
     <row r="60" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E60" s="9"/>
+      <c r="E60" s="7"/>
     </row>
     <row r="61" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E61" s="9"/>
+      <c r="E61" s="7"/>
     </row>
     <row r="62" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E62" s="9"/>
+      <c r="E62" s="7"/>
     </row>
     <row r="63" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E63" s="9"/>
+      <c r="E63" s="7"/>
     </row>
     <row r="64" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E64" s="9"/>
+      <c r="E64" s="7"/>
     </row>
     <row r="65" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E65" s="9"/>
+      <c r="E65" s="7"/>
     </row>
     <row r="66" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E66" s="9"/>
+      <c r="E66" s="7"/>
     </row>
     <row r="67" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E67" s="9"/>
+      <c r="E67" s="7"/>
     </row>
     <row r="68" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E68" s="9"/>
+      <c r="E68" s="7"/>
     </row>
     <row r="69" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E69" s="9"/>
+      <c r="E69" s="7"/>
     </row>
     <row r="70" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E70" s="9"/>
+      <c r="E70" s="7"/>
     </row>
     <row r="71" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E71" s="9"/>
+      <c r="E71" s="7"/>
     </row>
     <row r="72" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E72" s="9"/>
+      <c r="E72" s="7"/>
     </row>
     <row r="73" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E73" s="9"/>
+      <c r="E73" s="7"/>
     </row>
     <row r="74" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E74" s="9"/>
+      <c r="E74" s="7"/>
     </row>
     <row r="75" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E75" s="9"/>
+      <c r="E75" s="7"/>
     </row>
     <row r="76" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E76" s="9"/>
+      <c r="E76" s="7"/>
     </row>
     <row r="77" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E77" s="9"/>
+      <c r="E77" s="7"/>
     </row>
     <row r="78" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E78" s="9"/>
+      <c r="E78" s="7"/>
     </row>
     <row r="79" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E79" s="9"/>
+      <c r="E79" s="7"/>
     </row>
     <row r="80" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E80" s="9"/>
+      <c r="E80" s="7"/>
     </row>
     <row r="81" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E81" s="9"/>
+      <c r="E81" s="7"/>
     </row>
     <row r="82" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E82" s="9"/>
+      <c r="E82" s="7"/>
     </row>
     <row r="83" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E83" s="9"/>
+      <c r="E83" s="7"/>
     </row>
     <row r="84" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E84" s="9"/>
+      <c r="E84" s="7"/>
     </row>
     <row r="85" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E85" s="9"/>
+      <c r="E85" s="7"/>
     </row>
     <row r="86" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E86" s="9"/>
+      <c r="E86" s="7"/>
     </row>
     <row r="87" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E87" s="9"/>
+      <c r="E87" s="7"/>
     </row>
     <row r="88" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E88" s="9"/>
+      <c r="E88" s="7"/>
     </row>
     <row r="89" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E89" s="9"/>
+      <c r="E89" s="7"/>
     </row>
     <row r="90" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E90" s="9"/>
+      <c r="E90" s="7"/>
     </row>
     <row r="91" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E91" s="9"/>
+      <c r="E91" s="7"/>
     </row>
     <row r="92" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E92" s="9"/>
+      <c r="E92" s="7"/>
     </row>
     <row r="93" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E93" s="9"/>
+      <c r="E93" s="7"/>
     </row>
     <row r="94" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E94" s="9"/>
+      <c r="E94" s="7"/>
     </row>
     <row r="95" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E95" s="9"/>
+      <c r="E95" s="7"/>
     </row>
     <row r="96" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E96" s="9"/>
+      <c r="E96" s="7"/>
     </row>
     <row r="97" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E97" s="9"/>
+      <c r="E97" s="7"/>
     </row>
     <row r="98" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E98" s="9"/>
+      <c r="E98" s="7"/>
     </row>
     <row r="99" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E99" s="9"/>
+      <c r="E99" s="7"/>
     </row>
     <row r="100" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E100" s="9"/>
+      <c r="E100" s="7"/>
     </row>
     <row r="101" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E101" s="9"/>
+      <c r="E101" s="7"/>
     </row>
     <row r="102" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E102" s="9"/>
+      <c r="E102" s="7"/>
     </row>
     <row r="103" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E103" s="9"/>
+      <c r="E103" s="7"/>
     </row>
     <row r="104" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E104" s="9"/>
+      <c r="E104" s="7"/>
     </row>
     <row r="105" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E105" s="9"/>
+      <c r="E105" s="7"/>
     </row>
     <row r="106" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E106" s="9"/>
+      <c r="E106" s="7"/>
     </row>
     <row r="107" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E107" s="9"/>
+      <c r="E107" s="7"/>
     </row>
     <row r="108" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E108" s="9"/>
+      <c r="E108" s="7"/>
     </row>
     <row r="109" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E109" s="9"/>
+      <c r="E109" s="7"/>
     </row>
     <row r="110" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E110" s="9"/>
+      <c r="E110" s="7"/>
     </row>
     <row r="111" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E111" s="9"/>
+      <c r="E111" s="7"/>
     </row>
     <row r="112" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E112" s="9"/>
+      <c r="E112" s="7"/>
     </row>
     <row r="113" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E113" s="9"/>
+      <c r="E113" s="7"/>
     </row>
     <row r="114" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E114" s="9"/>
+      <c r="E114" s="7"/>
     </row>
     <row r="115" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E115" s="9"/>
+      <c r="E115" s="7"/>
     </row>
     <row r="116" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E116" s="9"/>
+      <c r="E116" s="7"/>
     </row>
     <row r="117" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E117" s="9"/>
+      <c r="E117" s="7"/>
     </row>
     <row r="118" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E118" s="9"/>
+      <c r="E118" s="7"/>
     </row>
     <row r="119" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E119" s="9"/>
+      <c r="E119" s="7"/>
     </row>
     <row r="120" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E120" s="9"/>
+      <c r="E120" s="7"/>
     </row>
     <row r="121" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E121" s="9"/>
+      <c r="E121" s="7"/>
     </row>
     <row r="122" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E122" s="9"/>
+      <c r="E122" s="7"/>
     </row>
     <row r="123" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E123" s="9"/>
+      <c r="E123" s="7"/>
     </row>
     <row r="124" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E124" s="9"/>
+      <c r="E124" s="7"/>
     </row>
     <row r="125" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E125" s="9"/>
+      <c r="E125" s="7"/>
     </row>
     <row r="126" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E126" s="9"/>
+      <c r="E126" s="7"/>
     </row>
     <row r="127" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E127" s="9"/>
+      <c r="E127" s="7"/>
     </row>
     <row r="128" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E128" s="9"/>
+      <c r="E128" s="7"/>
     </row>
     <row r="129" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E129" s="9"/>
+      <c r="E129" s="7"/>
     </row>
     <row r="130" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E130" s="9"/>
+      <c r="E130" s="7"/>
     </row>
     <row r="131" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E131" s="9"/>
+      <c r="E131" s="7"/>
     </row>
     <row r="132" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E132" s="9"/>
+      <c r="E132" s="7"/>
     </row>
     <row r="133" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E133" s="9"/>
+      <c r="E133" s="7"/>
     </row>
     <row r="134" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E134" s="9"/>
+      <c r="E134" s="7"/>
     </row>
     <row r="135" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E135" s="9"/>
+      <c r="E135" s="7"/>
     </row>
     <row r="136" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E136" s="9"/>
+      <c r="E136" s="7"/>
     </row>
     <row r="137" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E137" s="9"/>
+      <c r="E137" s="7"/>
     </row>
     <row r="138" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E138" s="9"/>
+      <c r="E138" s="7"/>
     </row>
     <row r="139" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E139" s="9"/>
+      <c r="E139" s="7"/>
     </row>
     <row r="140" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E140" s="9"/>
+      <c r="E140" s="7"/>
     </row>
     <row r="141" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E141" s="9"/>
+      <c r="E141" s="7"/>
     </row>
     <row r="142" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E142" s="9"/>
+      <c r="E142" s="7"/>
     </row>
     <row r="143" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E143" s="9"/>
+      <c r="E143" s="7"/>
     </row>
     <row r="144" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E144" s="9"/>
+      <c r="E144" s="7"/>
     </row>
     <row r="145" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E145" s="9"/>
+      <c r="E145" s="7"/>
     </row>
     <row r="146" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E146" s="9"/>
+      <c r="E146" s="7"/>
     </row>
     <row r="147" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E147" s="9"/>
+      <c r="E147" s="7"/>
     </row>
     <row r="148" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E148" s="9"/>
+      <c r="E148" s="7"/>
     </row>
     <row r="149" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E149" s="9"/>
+      <c r="E149" s="7"/>
     </row>
     <row r="150" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E150" s="9"/>
+      <c r="E150" s="7"/>
     </row>
     <row r="151" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E151" s="9"/>
+      <c r="E151" s="7"/>
     </row>
     <row r="152" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E152" s="9"/>
+      <c r="E152" s="7"/>
     </row>
     <row r="153" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E153" s="9"/>
+      <c r="E153" s="7"/>
     </row>
     <row r="154" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E154" s="9"/>
+      <c r="E154" s="7"/>
     </row>
     <row r="155" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E155" s="9"/>
+      <c r="E155" s="7"/>
     </row>
     <row r="156" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E156" s="9"/>
+      <c r="E156" s="7"/>
     </row>
     <row r="157" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E157" s="9"/>
+      <c r="E157" s="7"/>
     </row>
     <row r="158" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E158" s="9"/>
+      <c r="E158" s="7"/>
     </row>
     <row r="159" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E159" s="9"/>
+      <c r="E159" s="7"/>
     </row>
     <row r="160" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E160" s="9"/>
+      <c r="E160" s="7"/>
     </row>
     <row r="161" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E161" s="9"/>
+      <c r="E161" s="7"/>
     </row>
     <row r="162" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E162" s="9"/>
+      <c r="E162" s="7"/>
     </row>
     <row r="163" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E163" s="9"/>
+      <c r="E163" s="7"/>
     </row>
     <row r="164" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E164" s="9"/>
+      <c r="E164" s="7"/>
     </row>
     <row r="165" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E165" s="9"/>
+      <c r="E165" s="7"/>
     </row>
     <row r="166" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E166" s="9"/>
+      <c r="E166" s="7"/>
     </row>
     <row r="167" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E167" s="9"/>
+      <c r="E167" s="7"/>
     </row>
     <row r="168" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E168" s="9"/>
+      <c r="E168" s="7"/>
     </row>
     <row r="169" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E169" s="9"/>
+      <c r="E169" s="7"/>
     </row>
     <row r="170" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E170" s="9"/>
+      <c r="E170" s="7"/>
     </row>
     <row r="171" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E171" s="9"/>
+      <c r="E171" s="7"/>
     </row>
     <row r="172" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E172" s="9"/>
+      <c r="E172" s="7"/>
     </row>
     <row r="173" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E173" s="9"/>
+      <c r="E173" s="7"/>
     </row>
     <row r="174" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E174" s="9"/>
+      <c r="E174" s="7"/>
     </row>
     <row r="175" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E175" s="9"/>
+      <c r="E175" s="7"/>
     </row>
     <row r="176" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E176" s="9"/>
+      <c r="E176" s="7"/>
     </row>
     <row r="177" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E177" s="9"/>
+      <c r="E177" s="7"/>
     </row>
     <row r="178" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E178" s="9"/>
+      <c r="E178" s="7"/>
     </row>
     <row r="179" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E179" s="9"/>
+      <c r="E179" s="7"/>
     </row>
     <row r="180" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E180" s="9"/>
+      <c r="E180" s="7"/>
     </row>
     <row r="181" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E181" s="9"/>
+      <c r="E181" s="7"/>
     </row>
     <row r="182" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E182" s="9"/>
+      <c r="E182" s="7"/>
     </row>
     <row r="183" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E183" s="9"/>
+      <c r="E183" s="7"/>
     </row>
     <row r="184" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E184" s="9"/>
+      <c r="E184" s="7"/>
     </row>
     <row r="185" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E185" s="9"/>
+      <c r="E185" s="7"/>
     </row>
     <row r="186" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E186" s="9"/>
+      <c r="E186" s="7"/>
     </row>
     <row r="187" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E187" s="9"/>
+      <c r="E187" s="7"/>
     </row>
     <row r="188" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E188" s="9"/>
+      <c r="E188" s="7"/>
     </row>
     <row r="189" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E189" s="9"/>
+      <c r="E189" s="7"/>
     </row>
     <row r="190" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E190" s="9"/>
+      <c r="E190" s="7"/>
     </row>
     <row r="191" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E191" s="9"/>
+      <c r="E191" s="7"/>
     </row>
     <row r="192" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E192" s="9"/>
+      <c r="E192" s="7"/>
     </row>
     <row r="193" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E193" s="9"/>
+      <c r="E193" s="7"/>
     </row>
     <row r="194" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E194" s="9"/>
+      <c r="E194" s="7"/>
     </row>
     <row r="195" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E195" s="9"/>
+      <c r="E195" s="7"/>
     </row>
     <row r="196" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E196" s="9"/>
+      <c r="E196" s="7"/>
     </row>
     <row r="197" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E197" s="9"/>
+      <c r="E197" s="7"/>
     </row>
     <row r="198" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E198" s="9"/>
+      <c r="E198" s="7"/>
     </row>
     <row r="199" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E199" s="9"/>
+      <c r="E199" s="7"/>
     </row>
     <row r="200" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E200" s="9"/>
+      <c r="E200" s="7"/>
     </row>
     <row r="201" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E201" s="9"/>
+      <c r="E201" s="7"/>
     </row>
     <row r="202" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E202" s="9"/>
+      <c r="E202" s="7"/>
     </row>
     <row r="203" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E203" s="9"/>
+      <c r="E203" s="7"/>
     </row>
     <row r="204" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E204" s="9"/>
+      <c r="E204" s="7"/>
     </row>
     <row r="205" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E205" s="9"/>
+      <c r="E205" s="7"/>
     </row>
     <row r="206" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E206" s="9"/>
+      <c r="E206" s="7"/>
     </row>
     <row r="207" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E207" s="9"/>
+      <c r="E207" s="7"/>
     </row>
     <row r="208" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E208" s="9"/>
+      <c r="E208" s="7"/>
     </row>
     <row r="209" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E209" s="9"/>
+      <c r="E209" s="7"/>
     </row>
     <row r="210" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E210" s="9"/>
+      <c r="E210" s="7"/>
     </row>
     <row r="211" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E211" s="9"/>
+      <c r="E211" s="7"/>
     </row>
     <row r="212" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E212" s="9"/>
+      <c r="E212" s="7"/>
     </row>
     <row r="213" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E213" s="9"/>
+      <c r="E213" s="7"/>
     </row>
     <row r="214" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E214" s="9"/>
+      <c r="E214" s="7"/>
     </row>
     <row r="215" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E215" s="9"/>
+      <c r="E215" s="7"/>
     </row>
     <row r="216" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E216" s="9"/>
+      <c r="E216" s="7"/>
     </row>
     <row r="217" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E217" s="9"/>
+      <c r="E217" s="7"/>
     </row>
     <row r="218" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E218" s="9"/>
+      <c r="E218" s="7"/>
     </row>
     <row r="219" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E219" s="9"/>
+      <c r="E219" s="7"/>
     </row>
     <row r="220" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E220" s="9"/>
+      <c r="E220" s="7"/>
     </row>
     <row r="221" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E221" s="9"/>
+      <c r="E221" s="7"/>
     </row>
     <row r="222" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E222" s="9"/>
+      <c r="E222" s="7"/>
     </row>
     <row r="223" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E223" s="9"/>
+      <c r="E223" s="7"/>
     </row>
     <row r="224" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E224" s="9"/>
+      <c r="E224" s="7"/>
     </row>
     <row r="225" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E225" s="9"/>
+      <c r="E225" s="7"/>
     </row>
     <row r="226" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E226" s="9"/>
+      <c r="E226" s="7"/>
     </row>
     <row r="227" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E227" s="9"/>
+      <c r="E227" s="7"/>
     </row>
     <row r="228" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E228" s="9"/>
+      <c r="E228" s="7"/>
     </row>
     <row r="229" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E229" s="9"/>
+      <c r="E229" s="7"/>
     </row>
     <row r="230" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E230" s="9"/>
+      <c r="E230" s="7"/>
     </row>
     <row r="231" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E231" s="9"/>
+      <c r="E231" s="7"/>
     </row>
     <row r="232" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E232" s="9"/>
+      <c r="E232" s="7"/>
     </row>
     <row r="233" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E233" s="9"/>
+      <c r="E233" s="7"/>
     </row>
     <row r="234" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E234" s="9"/>
-    </row>
-    <row r="235" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E235" s="9"/>
-    </row>
-    <row r="236" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E236" s="9"/>
-    </row>
-    <row r="237" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E237" s="9"/>
-    </row>
-    <row r="238" spans="5:5" ht="15.75" customHeight="1">
-      <c r="E238" s="9"/>
-    </row>
+      <c r="E234" s="7"/>
+    </row>
+    <row r="235" spans="5:5" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="B44:F44"/>
     <mergeCell ref="B3:F4"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B5:F6"/>
-    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B43:F43"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B34:F34"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B15:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup scale="79" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="5" scale="79" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>